<commit_message>
Colleción de postman ejemplo y expiración del jwt extendida
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -31,10 +31,10 @@
     <t>user_id</t>
   </si>
   <si>
-    <t>2020-06-25T12:09:05.000Z</t>
-  </si>
-  <si>
-    <t>f1944946a7f15f7b36e465702ce0a244</t>
+    <t>2020-06-25T14:49:12.000Z</t>
+  </si>
+  <si>
+    <t>5b9e16f1a64d33e2f7abf2fce24e9b87</t>
   </si>
 </sst>
 </file>
@@ -74,7 +74,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -102,7 +102,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="0" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>6</v>
@@ -122,13 +122,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="0" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>30000</v>
+        <v>33000</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>30</v>
@@ -142,13 +142,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="0" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>20</v>
@@ -157,6 +157,306 @@
         <v>1</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>56000</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>32200</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>20030.5</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>50002</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>30200</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>20000</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>20000</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>20000</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>530000</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>22000</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>